<commit_message>
POD-Hybrid Automation Framework Model.xlsx updated
</commit_message>
<xml_diff>
--- a/POD-Hybrid Automation Framework Model.xlsx
+++ b/POD-Hybrid Automation Framework Model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="18195" windowHeight="8505" tabRatio="797"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="18195" windowHeight="8505" tabRatio="797" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Model" sheetId="7" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="97">
   <si>
     <t>Project</t>
   </si>
@@ -392,12 +392,6 @@
 2. Double clicking "RUN.BAT" file created &amp; containing Project Path &amp; "mvn clean install" command</t>
   </si>
   <si>
-    <t>Post installation of Jenkins on system, from Jenkins Portal:
-1. Using "Freestyle Project"
-OR
-2. Using "Maven Project"</t>
-  </si>
-  <si>
     <t>Option 1:
 Using Eclipse-"TestNG -
 TestRunner.XML" OR "Maven -
@@ -476,6 +470,62 @@
 cd &lt;projectworkplace location&gt;
 RUN.BAT</t>
     </r>
+  </si>
+  <si>
+    <t>Framework TechStack:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">TechStack used - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Java, Eclipse, Selenium, Maven &amp; POM.XML, TestNG, Log4J, Extent Reports, Jenkins, Git &amp; GitHub
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>Framework Key Features:</t>
+  </si>
+  <si>
+    <t>1. Framework for Web Automation -- Built on Open Source Technology Stack, as listed above
+2. Capable for Cross Browser, Data Driven &amp; Parallel Testing
+3. Suite Run possible - thru Eclipse, Maven, Jenkins
+4. Screen Capture for Failing Test Cases
+5. Reports in form of Log4J Logs, HTML based - TestNG &amp; Extent Reports
+6. CI/ CD Ready thru use of Maven, Jenkins &amp; Git-GitHub
+7. Scalable &amp; Customizable - Per Project Needs &amp; Requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post installation of Jenkins on system, from Jenkins Portal:
+1. Using "Freestyle Project"
+OR
+2. Using "Maven Project":
+2.1 POM.XML
+2.2 POM.XML &amp; GitHub URL
+</t>
   </si>
   <si>
     <r>
@@ -518,6 +568,17 @@
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Using POM.XML:</t>
+    </r>
+    <r>
+      <rPr>
         <u/>
         <sz val="11"/>
         <color theme="1"/>
@@ -542,51 +603,54 @@
     </r>
   </si>
   <si>
-    <t>Framework TechStack:</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">TechStack used - </t>
+      <t>Using POM.XML &amp; GitHub URL:</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Java, Eclipse, Selenium, Maven &amp; POM.XML, TestNG, Log4J, Extent Reports, Jenkins, Git &amp; GitHub
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
       <rPr>
-        <b/>
+        <u/>
         <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t/>
+      <t>New Item-&gt; Maven project-&gt;</t>
     </r>
-  </si>
-  <si>
-    <t>Framework Key Features:</t>
-  </si>
-  <si>
-    <t>1. Framework for Web Automation -- Built on Open Source Technology Stack, as listed above
-2. Capable for Cross Browser, Data Driven &amp; Parallel Testing
-3. Suite Run possible - thru Eclipse, Maven, Jenkins
-4. Screen Capture for Failing Test Cases
-5. Reports in form of Log4J Logs, HTML based - TestNG &amp; Extent Reports
-6. CI/ CD Ready thru use of Maven, Jenkins &amp; Git-GitHub
-7. Scalable &amp; Customizable - Per Project Needs &amp; Requirements</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:
+Source Code Management:
+Repository URL: https://github.com/kedardegaonkar/POD-HybridAutomationFrameworkModel.git
+Build Section:
+Root POM: POM.XML
+Goals and options: clean install</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1243,7 +1307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1351,9 +1415,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1378,6 +1439,12 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1420,6 +1487,33 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1513,38 +1607,20 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4782,8 +4858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4796,27 +4872,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="55"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="50"/>
+      <c r="D2" s="49"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -4831,7 +4907,7 @@
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="50"/>
+      <c r="D3" s="49"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
@@ -4846,7 +4922,7 @@
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="50"/>
+      <c r="D4" s="49"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -4861,7 +4937,7 @@
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
-      <c r="D5" s="50"/>
+      <c r="D5" s="49"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
@@ -4876,7 +4952,7 @@
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="50"/>
+      <c r="D6" s="49"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -4891,7 +4967,7 @@
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="50"/>
+      <c r="D7" s="49"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -4906,7 +4982,7 @@
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="50"/>
+      <c r="D8" s="49"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -4921,7 +4997,7 @@
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="50"/>
+      <c r="D9" s="49"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -4936,7 +5012,7 @@
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="50"/>
+      <c r="D10" s="49"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -4951,7 +5027,7 @@
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="50"/>
+      <c r="D11" s="49"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
@@ -4966,7 +5042,7 @@
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="50"/>
+      <c r="D12" s="49"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -4981,7 +5057,7 @@
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="50"/>
+      <c r="D13" s="49"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -4996,7 +5072,7 @@
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="50"/>
+      <c r="D14" s="49"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
@@ -5011,7 +5087,7 @@
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="50"/>
+      <c r="D15" s="49"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -5026,7 +5102,7 @@
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="50"/>
+      <c r="D16" s="49"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -5041,7 +5117,7 @@
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="50"/>
+      <c r="D17" s="49"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -5056,7 +5132,7 @@
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="50"/>
+      <c r="D18" s="49"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -5071,7 +5147,7 @@
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="50"/>
+      <c r="D19" s="49"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -5086,7 +5162,7 @@
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="50"/>
+      <c r="D20" s="49"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
@@ -5101,7 +5177,7 @@
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="50"/>
+      <c r="D21" s="49"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
@@ -5116,7 +5192,7 @@
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="50"/>
+      <c r="D22" s="49"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
@@ -5131,7 +5207,7 @@
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="50"/>
+      <c r="D23" s="49"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -5146,7 +5222,7 @@
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="50"/>
+      <c r="D24" s="49"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -5161,7 +5237,7 @@
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="50"/>
+      <c r="D25" s="49"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -5176,7 +5252,7 @@
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="50"/>
+      <c r="D26" s="49"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
@@ -5191,7 +5267,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="51"/>
+      <c r="D27" s="50"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
@@ -5217,7 +5293,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D3"/>
+      <selection sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5230,62 +5306,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="59"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="66"/>
+    </row>
+    <row r="3" spans="1:4" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="61"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="63"/>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="64" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
-    </row>
-    <row r="3" spans="1:4" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="59" t="s">
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="66"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="67" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="62"/>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="63" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="65"/>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="99" t="s">
-        <v>95</v>
-      </c>
-      <c r="B5" s="100"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="101"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="69"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="102"/>
-      <c r="B6" s="103"/>
-      <c r="C6" s="103"/>
-      <c r="D6" s="104"/>
+      <c r="A6" s="70"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="72"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="102"/>
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="104"/>
+      <c r="A7" s="70"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="72"/>
     </row>
     <row r="8" spans="1:4" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="105"/>
-      <c r="B8" s="106"/>
-      <c r="C8" s="106"/>
-      <c r="D8" s="107"/>
+      <c r="A8" s="73"/>
+      <c r="B8" s="74"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -5303,10 +5379,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5319,20 +5395,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="59"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="66"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
@@ -5431,12 +5507,12 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="63" t="s">
+      <c r="A10" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="65"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="66"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
@@ -5445,10 +5521,10 @@
       <c r="B11" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="75"/>
+      <c r="D11" s="85"/>
     </row>
     <row r="12" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31">
@@ -5457,10 +5533,10 @@
       <c r="B12" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="67"/>
+      <c r="D12" s="77"/>
     </row>
     <row r="13" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
@@ -5469,10 +5545,10 @@
       <c r="B13" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="68" t="s">
+      <c r="C13" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="69"/>
+      <c r="D13" s="79"/>
     </row>
     <row r="14" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
@@ -5481,10 +5557,10 @@
       <c r="B14" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="70" t="s">
+      <c r="C14" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="71"/>
+      <c r="D14" s="81"/>
     </row>
     <row r="15" spans="1:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
@@ -5493,18 +5569,18 @@
       <c r="B15" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="72" t="s">
+      <c r="C15" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="73"/>
+      <c r="D15" s="83"/>
     </row>
     <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="63" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="65"/>
+      <c r="A16" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="65"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="66"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
@@ -5513,61 +5589,72 @@
       <c r="B17" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="74" t="s">
+      <c r="C17" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="75"/>
+      <c r="D17" s="85"/>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="31">
         <v>1</v>
       </c>
-      <c r="B18" s="97" t="s">
+      <c r="B18" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="76" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="77"/>
+    </row>
+    <row r="19" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="52">
+        <v>2</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="78" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="79"/>
+    </row>
+    <row r="20" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="52">
+        <v>3</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="80" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="81"/>
+    </row>
+    <row r="21" spans="1:4" ht="363" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="92">
+        <v>4</v>
+      </c>
+      <c r="B21" s="109" t="s">
         <v>87</v>
       </c>
-      <c r="C18" s="66" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="67"/>
-    </row>
-    <row r="19" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="41">
-        <v>2</v>
-      </c>
-      <c r="B19" s="40" t="s">
-        <v>84</v>
-      </c>
-      <c r="C19" s="68" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="69"/>
-    </row>
-    <row r="20" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="41">
-        <v>3</v>
-      </c>
-      <c r="B20" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" s="70" t="s">
-        <v>90</v>
-      </c>
-      <c r="D20" s="71"/>
-    </row>
-    <row r="21" spans="1:4" ht="365.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10">
-        <v>4</v>
-      </c>
-      <c r="B21" s="98" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" s="72" t="s">
-        <v>91</v>
-      </c>
-      <c r="D21" s="73"/>
+      <c r="C21" s="80" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="81"/>
+    </row>
+    <row r="22" spans="1:4" ht="141" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="108"/>
+      <c r="B22" s="107"/>
+      <c r="C22" s="110" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="111"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="17">
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A21:A22"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="C17:D17"/>
@@ -5592,8 +5679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:B31"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5606,20 +5693,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="59"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="66"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
@@ -5650,11 +5737,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="82">
+      <c r="A5" s="92">
         <v>2</v>
       </c>
-      <c r="B5" s="87" t="s">
-        <v>82</v>
+      <c r="B5" s="97" t="s">
+        <v>81</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>2</v>
@@ -5664,18 +5751,18 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="82"/>
-      <c r="B6" s="88"/>
+      <c r="A6" s="92"/>
+      <c r="B6" s="98"/>
       <c r="C6" s="39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="82"/>
-      <c r="B7" s="88"/>
+      <c r="A7" s="92"/>
+      <c r="B7" s="98"/>
       <c r="C7" s="16" t="s">
         <v>7</v>
       </c>
@@ -5684,8 +5771,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="82"/>
-      <c r="B8" s="88"/>
+      <c r="A8" s="92"/>
+      <c r="B8" s="98"/>
       <c r="C8" s="16" t="s">
         <v>3</v>
       </c>
@@ -5697,8 +5784,8 @@
       <c r="A9" s="15">
         <v>3</v>
       </c>
-      <c r="B9" s="48" t="s">
-        <v>83</v>
+      <c r="B9" s="47" t="s">
+        <v>82</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>10</v>
@@ -5708,64 +5795,64 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="83">
+      <c r="A10" s="93">
         <v>4</v>
       </c>
-      <c r="B10" s="84" t="s">
+      <c r="B10" s="94" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="71" t="s">
+      <c r="D10" s="81" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="82"/>
-      <c r="B11" s="85"/>
+      <c r="A11" s="92"/>
+      <c r="B11" s="95"/>
       <c r="C11" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="71"/>
+      <c r="D11" s="81"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="82"/>
-      <c r="B12" s="85"/>
+      <c r="A12" s="92"/>
+      <c r="B12" s="95"/>
       <c r="C12" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="71"/>
+      <c r="D12" s="81"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="82"/>
-      <c r="B13" s="85"/>
+      <c r="A13" s="92"/>
+      <c r="B13" s="95"/>
       <c r="C13" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="71"/>
+      <c r="D13" s="81"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="82"/>
-      <c r="B14" s="85"/>
+      <c r="A14" s="92"/>
+      <c r="B14" s="95"/>
       <c r="C14" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="71"/>
+      <c r="D14" s="81"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="82"/>
-      <c r="B15" s="86"/>
+      <c r="A15" s="92"/>
+      <c r="B15" s="96"/>
       <c r="C15" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="71"/>
+      <c r="D15" s="81"/>
     </row>
     <row r="16" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>5</v>
       </c>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="48" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="16" t="s">
@@ -5776,64 +5863,64 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="83">
+      <c r="A17" s="93">
         <v>6.1</v>
       </c>
-      <c r="B17" s="89" t="s">
+      <c r="B17" s="99" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="71" t="s">
+      <c r="D17" s="81" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="83"/>
-      <c r="B18" s="89"/>
+      <c r="A18" s="93"/>
+      <c r="B18" s="99"/>
       <c r="C18" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="71"/>
+      <c r="D18" s="81"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="83"/>
-      <c r="B19" s="89"/>
+      <c r="A19" s="93"/>
+      <c r="B19" s="99"/>
       <c r="C19" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="71"/>
+      <c r="D19" s="81"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="83"/>
-      <c r="B20" s="89"/>
+      <c r="A20" s="93"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="71"/>
+      <c r="D20" s="81"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="83"/>
-      <c r="B21" s="89"/>
+      <c r="A21" s="93"/>
+      <c r="B21" s="99"/>
       <c r="C21" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="71"/>
+      <c r="D21" s="81"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="83"/>
-      <c r="B22" s="89"/>
+      <c r="A22" s="93"/>
+      <c r="B22" s="99"/>
       <c r="C22" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="71"/>
+      <c r="D22" s="81"/>
     </row>
     <row r="23" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>6.2</v>
       </c>
-      <c r="B23" s="90" t="s">
+      <c r="B23" s="100" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -5847,7 +5934,7 @@
       <c r="A24" s="17">
         <v>6.3</v>
       </c>
-      <c r="B24" s="91"/>
+      <c r="B24" s="101"/>
       <c r="C24" s="40" t="s">
         <v>23</v>
       </c>
@@ -5859,8 +5946,8 @@
       <c r="A25" s="17">
         <v>6.4</v>
       </c>
-      <c r="B25" s="48" t="s">
-        <v>83</v>
+      <c r="B25" s="47" t="s">
+        <v>82</v>
       </c>
       <c r="C25" s="40" t="s">
         <v>21</v>
@@ -5873,11 +5960,11 @@
       <c r="A26" s="15">
         <v>7.1</v>
       </c>
-      <c r="B26" s="76" t="s">
+      <c r="B26" s="86" t="s">
         <v>31</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>72</v>
@@ -5887,7 +5974,7 @@
       <c r="A27" s="15">
         <v>7.2</v>
       </c>
-      <c r="B27" s="77"/>
+      <c r="B27" s="87"/>
       <c r="C27" s="19" t="s">
         <v>71</v>
       </c>
@@ -5895,24 +5982,24 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>7.3</v>
       </c>
-      <c r="B28" s="78"/>
+      <c r="B28" s="88"/>
       <c r="C28" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>8</v>
       </c>
-      <c r="B29" s="48" t="s">
-        <v>83</v>
+      <c r="B29" s="47" t="s">
+        <v>82</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>30</v>
@@ -5922,38 +6009,38 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="45">
+      <c r="A30" s="44">
         <v>9.1</v>
       </c>
-      <c r="B30" s="92" t="s">
+      <c r="B30" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="46" t="s">
+      <c r="C30" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="47" t="s">
+    </row>
+    <row r="31" spans="1:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="44">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="B31" s="103"/>
+      <c r="C31" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="46" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="45">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="B31" s="93"/>
-      <c r="C31" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="47" t="s">
-        <v>80</v>
-      </c>
-    </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="79" t="s">
+      <c r="A32" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="80"/>
-      <c r="C32" s="80"/>
-      <c r="D32" s="81"/>
+      <c r="B32" s="90"/>
+      <c r="C32" s="90"/>
+      <c r="D32" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -5991,32 +6078,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="104" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="96"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="106"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="65"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="66"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="42"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="43"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>

</xml_diff>

<commit_message>
Updated POD xls file and TC Classes for ExtentReport Steps
</commit_message>
<xml_diff>
--- a/POD-Hybrid Automation Framework Model.xlsx
+++ b/POD-Hybrid Automation Framework Model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="18195" windowHeight="8505" tabRatio="797" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="18195" windowHeight="8505" tabRatio="797" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Model" sheetId="7" r:id="rId1"/>
@@ -298,21 +298,6 @@
       </rPr>
       <t xml:space="preserve"> -- Page Object Classes &amp; Test Case Classes for other Pages/ Functionalities can be created in similar way, as explained above.</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Contains:
-1. Object for ReadConfig.java (to get BaseURL, Login Credentials, Browser Driver Exe &amp; Test Data Xlsx File Paths), WebDriver, Log4j, TestData File
-2. @Parameters ("browser")
-3. @BeforeClass (for Browser Initialization)
-4. @AfterClass (for Browser Close, Quit)
-5. Common Util Methods </t>
-  </si>
-  <si>
-    <t>1. Extends Base Class - for Login Credentials
-2. Object for each Page Object Class, required for Test Case Execution
-3. @Test for actual test 
-4. Call to Common Util Methods (as required) from BaseClass.java
-5. Test Case specific Methods in each Test Case</t>
   </si>
   <si>
     <t>1. Generates Test Result Reports in Extent Reports - HTML format
@@ -651,6 +636,22 @@
 Root POM: POM.XML
 Goals and options: clean install</t>
     </r>
+  </si>
+  <si>
+    <t>1. Extends Base Class - for Login Credentials
+2. Object for each Page Object Class, required for Test Case Execution
+3. import UtilsClasses.ExtentReport;
+4. @Test for actual test 
+5. Call to Common Util Methods (as required) from BaseClass.java
+6. Test Case specific Methods in each Test Case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contains:
+1. Object for ReadConfig.java (to get BaseURL, Login Credentials, Browser Driver Exe &amp; Test Data Xlsx File Paths), WebDriver, Log4j, TestData Xlsx File
+2. @Parameters ("browser")
+3. @BeforeClass (for Browser Initialization)
+4. @AfterClass (for Browser Close, Quit)
+5. Common Util Methods </t>
   </si>
 </sst>
 </file>
@@ -1544,6 +1545,24 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1563,9 +1582,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1606,21 +1622,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5315,7 +5316,7 @@
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="64" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
@@ -5323,7 +5324,7 @@
     </row>
     <row r="3" spans="1:4" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="60" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B3" s="61"/>
       <c r="C3" s="62"/>
@@ -5331,7 +5332,7 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="64" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B4" s="65"/>
       <c r="C4" s="65"/>
@@ -5339,7 +5340,7 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="67" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B5" s="68"/>
       <c r="C5" s="68"/>
@@ -5381,8 +5382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:D14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5576,7 +5577,7 @@
     </row>
     <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="64" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B16" s="65"/>
       <c r="C16" s="65"/>
@@ -5599,10 +5600,10 @@
         <v>1</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C18" s="76" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D18" s="77"/>
     </row>
@@ -5611,10 +5612,10 @@
         <v>2</v>
       </c>
       <c r="B19" s="40" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C19" s="78" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D19" s="79"/>
     </row>
@@ -5623,32 +5624,32 @@
         <v>3</v>
       </c>
       <c r="B20" s="40" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C20" s="80" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D20" s="81"/>
     </row>
     <row r="21" spans="1:4" ht="363" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="92">
+      <c r="A21" s="90">
         <v>4</v>
       </c>
-      <c r="B21" s="109" t="s">
-        <v>87</v>
+      <c r="B21" s="88" t="s">
+        <v>85</v>
       </c>
       <c r="C21" s="80" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D21" s="81"/>
     </row>
     <row r="22" spans="1:4" ht="141" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="108"/>
-      <c r="B22" s="107"/>
-      <c r="C22" s="110" t="s">
-        <v>96</v>
-      </c>
-      <c r="D22" s="111"/>
+      <c r="A22" s="91"/>
+      <c r="B22" s="89"/>
+      <c r="C22" s="86" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -5679,8 +5680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5737,11 +5738,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="92">
+      <c r="A5" s="90">
         <v>2</v>
       </c>
-      <c r="B5" s="97" t="s">
-        <v>81</v>
+      <c r="B5" s="102" t="s">
+        <v>79</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>2</v>
@@ -5751,18 +5752,18 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="92"/>
-      <c r="B6" s="98"/>
+      <c r="A6" s="90"/>
+      <c r="B6" s="103"/>
       <c r="C6" s="39" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="92"/>
-      <c r="B7" s="98"/>
+      <c r="A7" s="90"/>
+      <c r="B7" s="103"/>
       <c r="C7" s="16" t="s">
         <v>7</v>
       </c>
@@ -5771,8 +5772,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="92"/>
-      <c r="B8" s="98"/>
+      <c r="A8" s="90"/>
+      <c r="B8" s="103"/>
       <c r="C8" s="16" t="s">
         <v>3</v>
       </c>
@@ -5785,7 +5786,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="47" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>10</v>
@@ -5795,10 +5796,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="93">
+      <c r="A10" s="98">
         <v>4</v>
       </c>
-      <c r="B10" s="94" t="s">
+      <c r="B10" s="99" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="16" t="s">
@@ -5809,40 +5810,40 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="92"/>
-      <c r="B11" s="95"/>
+      <c r="A11" s="90"/>
+      <c r="B11" s="100"/>
       <c r="C11" s="16" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="81"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="92"/>
-      <c r="B12" s="95"/>
+      <c r="A12" s="90"/>
+      <c r="B12" s="100"/>
       <c r="C12" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D12" s="81"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="92"/>
-      <c r="B13" s="95"/>
+      <c r="A13" s="90"/>
+      <c r="B13" s="100"/>
       <c r="C13" s="37" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D13" s="81"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="92"/>
-      <c r="B14" s="95"/>
+      <c r="A14" s="90"/>
+      <c r="B14" s="100"/>
       <c r="C14" s="37" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="81"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="92"/>
-      <c r="B15" s="96"/>
+      <c r="A15" s="90"/>
+      <c r="B15" s="101"/>
       <c r="C15" s="16" t="s">
         <v>17</v>
       </c>
@@ -5859,58 +5860,58 @@
         <v>11</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="93">
+      <c r="A17" s="98">
         <v>6.1</v>
       </c>
-      <c r="B17" s="99" t="s">
+      <c r="B17" s="104" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="81" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="93"/>
-      <c r="B18" s="99"/>
+      <c r="A18" s="98"/>
+      <c r="B18" s="104"/>
       <c r="C18" s="16" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="81"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="93"/>
-      <c r="B19" s="99"/>
+      <c r="A19" s="98"/>
+      <c r="B19" s="104"/>
       <c r="C19" s="16" t="s">
         <v>55</v>
       </c>
       <c r="D19" s="81"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="93"/>
-      <c r="B20" s="99"/>
+      <c r="A20" s="98"/>
+      <c r="B20" s="104"/>
       <c r="C20" s="16" t="s">
         <v>56</v>
       </c>
       <c r="D20" s="81"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="93"/>
-      <c r="B21" s="99"/>
+      <c r="A21" s="98"/>
+      <c r="B21" s="104"/>
       <c r="C21" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="81"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="93"/>
-      <c r="B22" s="99"/>
+    <row r="22" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="98"/>
+      <c r="B22" s="104"/>
       <c r="C22" s="16" t="s">
         <v>17</v>
       </c>
@@ -5920,7 +5921,7 @@
       <c r="A23" s="17">
         <v>6.2</v>
       </c>
-      <c r="B23" s="100" t="s">
+      <c r="B23" s="105" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -5934,7 +5935,7 @@
       <c r="A24" s="17">
         <v>6.3</v>
       </c>
-      <c r="B24" s="101"/>
+      <c r="B24" s="106"/>
       <c r="C24" s="40" t="s">
         <v>23</v>
       </c>
@@ -5947,7 +5948,7 @@
         <v>6.4</v>
       </c>
       <c r="B25" s="47" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C25" s="40" t="s">
         <v>21</v>
@@ -5960,38 +5961,38 @@
       <c r="A26" s="15">
         <v>7.1</v>
       </c>
-      <c r="B26" s="86" t="s">
+      <c r="B26" s="92" t="s">
         <v>31</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>7.2</v>
       </c>
-      <c r="B27" s="87"/>
+      <c r="B27" s="93"/>
       <c r="C27" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="18" t="s">
         <v>71</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>7.3</v>
       </c>
-      <c r="B28" s="88"/>
+      <c r="B28" s="94"/>
       <c r="C28" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5999,48 +6000,48 @@
         <v>8</v>
       </c>
       <c r="B29" s="47" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>30</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="44">
         <v>9.1</v>
       </c>
-      <c r="B30" s="102" t="s">
+      <c r="B30" s="107" t="s">
         <v>20</v>
       </c>
       <c r="C30" s="45" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D30" s="46" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="44">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B31" s="103"/>
+      <c r="B31" s="108"/>
       <c r="C31" s="45" t="s">
         <v>45</v>
       </c>
       <c r="D31" s="46" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="89" t="s">
+      <c r="A32" s="95" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="90"/>
-      <c r="C32" s="90"/>
-      <c r="D32" s="91"/>
+      <c r="B32" s="96"/>
+      <c r="C32" s="96"/>
+      <c r="D32" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -6078,14 +6079,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="106"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="111"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="64" t="s">

</xml_diff>